<commit_message>
add Red and Blue LED
</commit_message>
<xml_diff>
--- a/鸽子喂料机/STM32喂料机引脚使用表.xlsx
+++ b/鸽子喂料机/STM32喂料机引脚使用表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>STM32引脚使用表</t>
   </si>
@@ -75,19 +75,25 @@
     <t>USART3_RX</t>
   </si>
   <si>
-    <t>RX3</t>
+    <t>伺服电机RX3</t>
   </si>
   <si>
     <t>A8</t>
   </si>
   <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>红灯</t>
+  </si>
+  <si>
     <t>B10</t>
   </si>
   <si>
     <t>USART3_TX</t>
   </si>
   <si>
-    <t>TX3</t>
+    <t>伺服电机TX3</t>
   </si>
   <si>
     <t>A9</t>
@@ -99,6 +105,12 @@
     <t>B1</t>
   </si>
   <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>蓝灯</t>
+  </si>
+  <si>
     <t>A10</t>
   </si>
   <si>
@@ -150,6 +162,9 @@
     <t>HCSR04_TRIG1</t>
   </si>
   <si>
+    <t>超声波1</t>
+  </si>
+  <si>
     <t>A5</t>
   </si>
   <si>
@@ -165,6 +180,9 @@
     <t>HCSR04_TRIG2</t>
   </si>
   <si>
+    <t>超声波2</t>
+  </si>
+  <si>
     <t>A4</t>
   </si>
   <si>
@@ -180,13 +198,16 @@
     <t>HCSR04_TRIG3</t>
   </si>
   <si>
+    <t>超声波3</t>
+  </si>
+  <si>
     <t>A3</t>
   </si>
   <si>
     <t>USART2_RX</t>
   </si>
   <si>
-    <t>RX2</t>
+    <t>伺服电机RX2</t>
   </si>
   <si>
     <t>B5</t>
@@ -195,13 +216,16 @@
     <t>HCSR04_TRIG4</t>
   </si>
   <si>
+    <t>超声波4</t>
+  </si>
+  <si>
     <t>A2</t>
   </si>
   <si>
     <t>USART2_TX</t>
   </si>
   <si>
-    <t>TX2</t>
+    <t>伺服电机TX2</t>
   </si>
   <si>
     <t>B6</t>
@@ -260,10 +284,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -295,8 +319,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,6 +356,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -339,14 +440,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -355,35 +448,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -391,46 +455,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -441,13 +465,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,13 +579,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,19 +627,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,127 +639,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,54 +656,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -702,7 +678,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,13 +709,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -740,149 +764,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -891,9 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1249,7 +1270,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1271,14 +1292,14 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1286,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1294,14 +1315,14 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1309,7 +1330,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1317,14 +1338,14 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1332,7 +1353,7 @@
         <v>11</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1340,14 +1361,14 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1355,7 +1376,7 @@
         <v>15</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1367,297 +1388,327 @@
         <v>18</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="4" t="s">
-        <v>23</v>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F8" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
+      <c r="D9" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="4" t="s">
-        <v>33</v>
+      <c r="I9" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="4" t="s">
-        <v>36</v>
+      <c r="D10" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="4" t="s">
-        <v>38</v>
+      <c r="I10" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="4" t="s">
-        <v>41</v>
+      <c r="D11" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="4" t="s">
-        <v>46</v>
+      <c r="D12" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8">
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="3"/>
       <c r="F17" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="F18" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H18" s="1"/>
+      <c r="I18" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="D19" s="3"/>
       <c r="F19" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3" t="s">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="3"/>
+      <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="D20" s="3"/>
       <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3" t="s">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="3"/>
+      <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3" t="s">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="3"/>
+      <c r="J21" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="46">

</xml_diff>